<commit_message>
Combo Box - Binding
Expirare Guna Framework
</commit_message>
<xml_diff>
--- a/2. Documentatie/Baza de date.xlsx
+++ b/2. Documentatie/Baza de date.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Schema BD" sheetId="6" r:id="rId1"/>
     <sheet name="Schema POO" sheetId="7" r:id="rId2"/>
+    <sheet name="Schema POO (2)" sheetId="8" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="124">
   <si>
     <t>Adresa</t>
   </si>
@@ -704,12 +705,30 @@
       <t xml:space="preserve"> Adresa</t>
     </r>
   </si>
+  <si>
+    <t>regiuneRecenzata</t>
+  </si>
+  <si>
+    <t>judetRecenzat</t>
+  </si>
+  <si>
+    <t>localirtateRecenzata</t>
+  </si>
+  <si>
+    <t>List&lt;String&gt;</t>
+  </si>
+  <si>
+    <t>listaRecenzati</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -827,6 +846,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="12">
     <fill>
@@ -1191,7 +1218,7 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1216,33 +1243,6 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1267,11 +1267,51 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="10" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="11" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="11" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="10" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1279,14 +1319,17 @@
     <xf numFmtId="0" fontId="6" fillId="9" borderId="11" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="10" xfId="10" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="20" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="11" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="20" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="10" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1295,14 +1338,11 @@
     <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -2188,10 +2228,10 @@
       <c r="N8" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="O8" s="16" t="s">
+      <c r="O8" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="P8" s="16"/>
+      <c r="P8" s="27"/>
       <c r="Q8" s="1" t="s">
         <v>45</v>
       </c>
@@ -2436,8 +2476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2457,543 +2497,594 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="C1" s="42"/>
-      <c r="H1" s="39" t="s">
+      <c r="C1" s="48"/>
+      <c r="H1" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="I1" s="39"/>
-      <c r="L1" s="39" t="s">
+      <c r="I1" s="42"/>
+      <c r="L1" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="M1" s="39"/>
+      <c r="M1" s="42"/>
     </row>
     <row r="2" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="H2" s="33" t="s">
+      <c r="C2" s="44"/>
+      <c r="H2" s="43" t="s">
         <v>94</v>
       </c>
-      <c r="I2" s="34"/>
-      <c r="L2" s="43" t="s">
+      <c r="I2" s="44"/>
+      <c r="L2" s="45" t="s">
         <v>117</v>
       </c>
-      <c r="M2" s="34"/>
+      <c r="M2" s="44"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="H3" s="29" t="s">
+      <c r="H3" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="I3" s="28" t="s">
+      <c r="I3" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="L3" s="27" t="s">
+      <c r="L3" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="M3" s="28" t="s">
+      <c r="M3" s="19" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="H4" s="29" t="s">
+      <c r="H4" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="I4" s="30" t="s">
+      <c r="I4" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="L4" s="29" t="s">
+      <c r="L4" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="M4" s="30" t="s">
+      <c r="M4" s="21" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="H5" s="29" t="s">
+      <c r="H5" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="I5" s="30" t="s">
+      <c r="I5" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="L5" s="29" t="s">
+      <c r="L5" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="M5" s="30" t="s">
+      <c r="M5" s="21" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="6" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="C6" s="32" t="s">
+      <c r="C6" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="31" t="s">
+      <c r="H6" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="I6" s="32" t="s">
+      <c r="I6" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="L6" s="29" t="s">
+      <c r="L6" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="M6" s="30" t="s">
+      <c r="M6" s="21" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="C7" s="18"/>
-      <c r="H7" s="17" t="s">
+      <c r="C7" s="33"/>
+      <c r="H7" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="I7" s="18"/>
-      <c r="L7" s="29" t="s">
+      <c r="I7" s="33"/>
+      <c r="L7" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="M7" s="44" t="s">
+      <c r="M7" s="25" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="C8" s="20"/>
-      <c r="H8" s="19" t="s">
+      <c r="C8" s="31"/>
+      <c r="H8" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="I8" s="20"/>
-      <c r="L8" s="29" t="s">
+      <c r="I8" s="31"/>
+      <c r="L8" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="M8" s="30" t="s">
+      <c r="M8" s="21" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="C9" s="22"/>
-      <c r="H9" s="21" t="s">
+      <c r="C9" s="35"/>
+      <c r="H9" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="I9" s="22"/>
-      <c r="L9" s="29" t="s">
+      <c r="I9" s="35"/>
+      <c r="L9" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="M9" s="30" t="s">
+      <c r="M9" s="21" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="10" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="C10" s="24"/>
-      <c r="H10" s="23" t="s">
+      <c r="C10" s="37"/>
+      <c r="H10" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="I10" s="24"/>
-      <c r="L10" s="29" t="s">
+      <c r="I10" s="37"/>
+      <c r="L10" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="M10" s="30" t="s">
+      <c r="M10" s="21" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="11" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="C11" s="26"/>
-      <c r="L11" s="31" t="s">
+      <c r="C11" s="39"/>
+      <c r="L11" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="M11" s="45" t="s">
+      <c r="M11" s="26" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="12" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="35" t="s">
+      <c r="B12" s="40" t="s">
         <v>82</v>
       </c>
-      <c r="C12" s="36"/>
-      <c r="L12" s="17" t="s">
+      <c r="C12" s="41"/>
+      <c r="L12" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="M12" s="18"/>
+      <c r="M12" s="33"/>
     </row>
     <row r="13" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="37" t="s">
+      <c r="B13" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="C13" s="38"/>
-      <c r="H13" s="39" t="s">
+      <c r="C13" s="29"/>
+      <c r="H13" s="42" t="s">
         <v>92</v>
       </c>
-      <c r="I13" s="39"/>
-      <c r="L13" s="19" t="s">
+      <c r="I13" s="42"/>
+      <c r="L13" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="M13" s="20"/>
+      <c r="M13" s="31"/>
     </row>
     <row r="14" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H14" s="43" t="s">
+      <c r="H14" s="45" t="s">
         <v>98</v>
       </c>
-      <c r="I14" s="34"/>
-      <c r="L14" s="21" t="s">
+      <c r="I14" s="44"/>
+      <c r="L14" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="M14" s="22"/>
+      <c r="M14" s="35"/>
     </row>
     <row r="15" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H15" s="29" t="s">
+      <c r="H15" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="I15" s="28" t="s">
+      <c r="I15" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="L15" s="23" t="s">
+      <c r="L15" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="M15" s="24"/>
+      <c r="M15" s="37"/>
     </row>
     <row r="16" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="C16" s="42"/>
-      <c r="H16" s="29" t="s">
+      <c r="C16" s="48"/>
+      <c r="H16" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="I16" s="30" t="s">
+      <c r="I16" s="21" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="17" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="33" t="s">
+      <c r="B17" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="C17" s="34"/>
-      <c r="H17" s="29" t="s">
+      <c r="C17" s="44"/>
+      <c r="H17" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="I17" s="30" t="s">
+      <c r="I17" s="21" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="18" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="28" t="s">
+      <c r="C18" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="H18" s="17" t="s">
+      <c r="H18" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="I18" s="18"/>
-      <c r="L18" s="39" t="s">
+      <c r="I18" s="33"/>
+      <c r="L18" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="M18" s="39"/>
+      <c r="M18" s="42"/>
     </row>
     <row r="19" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="30" t="s">
+      <c r="C19" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="H19" s="19" t="s">
+      <c r="H19" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="I19" s="20"/>
-      <c r="L19" s="33" t="s">
+      <c r="I19" s="31"/>
+      <c r="L19" s="43" t="s">
         <v>116</v>
       </c>
-      <c r="M19" s="34"/>
+      <c r="M19" s="44"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B20" s="29" t="s">
+      <c r="B20" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="30" t="s">
+      <c r="C20" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="H20" s="21" t="s">
+      <c r="H20" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="I20" s="22"/>
-      <c r="L20" s="29" t="s">
+      <c r="I20" s="35"/>
+      <c r="L20" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="M20" s="30" t="s">
+      <c r="M20" s="21" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="21" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="31" t="s">
+      <c r="B21" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="C21" s="32" t="s">
+      <c r="C21" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="H21" s="23" t="s">
+      <c r="H21" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="I21" s="24"/>
-      <c r="L21" s="29" t="s">
+      <c r="I21" s="37"/>
+      <c r="L21" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="M21" s="30" t="s">
+      <c r="M21" s="21" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="22" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="H22" s="25" t="s">
+      <c r="C22" s="33"/>
+      <c r="H22" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="I22" s="26"/>
-      <c r="L22" s="17" t="s">
+      <c r="I22" s="39"/>
+      <c r="L22" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="M22" s="18"/>
+      <c r="M22" s="33"/>
     </row>
     <row r="23" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="19" t="s">
+      <c r="B23" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="C23" s="20"/>
-      <c r="H23" s="35" t="s">
+      <c r="C23" s="31"/>
+      <c r="H23" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="I23" s="36"/>
-      <c r="L23" s="19" t="s">
+      <c r="I23" s="41"/>
+      <c r="L23" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="M23" s="20"/>
+      <c r="M23" s="31"/>
     </row>
     <row r="24" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="19" t="s">
+      <c r="B24" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="C24" s="20"/>
-      <c r="H24" s="37" t="s">
+      <c r="C24" s="31"/>
+      <c r="H24" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="I24" s="38"/>
-      <c r="L24" s="21" t="s">
+      <c r="I24" s="29"/>
+      <c r="L24" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="M24" s="22"/>
+      <c r="M24" s="35"/>
     </row>
     <row r="25" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="21" t="s">
+      <c r="B25" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="C25" s="22"/>
-      <c r="L25" s="23" t="s">
+      <c r="C25" s="35"/>
+      <c r="L25" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="M25" s="24"/>
+      <c r="M25" s="37"/>
     </row>
     <row r="26" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="23" t="s">
+      <c r="B26" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="C26" s="24"/>
+      <c r="C26" s="37"/>
     </row>
     <row r="27" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="25" t="s">
+      <c r="B27" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="C27" s="26"/>
-      <c r="H27" s="39" t="s">
+      <c r="C27" s="39"/>
+      <c r="H27" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="I27" s="39"/>
+      <c r="I27" s="42"/>
     </row>
     <row r="28" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="40"/>
-      <c r="C28" s="40"/>
-      <c r="H28" s="33" t="s">
+      <c r="B28" s="46"/>
+      <c r="C28" s="46"/>
+      <c r="H28" s="43" t="s">
         <v>102</v>
       </c>
-      <c r="I28" s="34"/>
-      <c r="L28" s="39" t="s">
+      <c r="I28" s="44"/>
+      <c r="L28" s="42" t="s">
         <v>104</v>
       </c>
-      <c r="M28" s="39"/>
+      <c r="M28" s="42"/>
     </row>
     <row r="29" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="H29" s="25" t="s">
+      <c r="B29" s="46"/>
+      <c r="C29" s="46"/>
+      <c r="H29" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="I29" s="26"/>
-      <c r="L29" s="33" t="s">
+      <c r="I29" s="39"/>
+      <c r="L29" s="43" t="s">
         <v>101</v>
       </c>
-      <c r="M29" s="34"/>
+      <c r="M29" s="44"/>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="L30" s="27" t="s">
+      <c r="L30" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="M30" s="28" t="s">
+      <c r="M30" s="19" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="31" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="L31" s="29" t="s">
+      <c r="L31" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="M31" s="30" t="s">
+      <c r="M31" s="21" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="32" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="41" t="s">
+      <c r="B32" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="C32" s="42"/>
-      <c r="L32" s="29" t="s">
+      <c r="C32" s="48"/>
+      <c r="L32" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="M32" s="30" t="s">
+      <c r="M32" s="21" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="33" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="33" t="s">
+      <c r="B33" s="43" t="s">
         <v>89</v>
       </c>
-      <c r="C33" s="34"/>
-      <c r="L33" s="31" t="s">
+      <c r="C33" s="44"/>
+      <c r="L33" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="M33" s="32" t="s">
+      <c r="M33" s="23" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B34" s="27" t="s">
+      <c r="B34" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C34" s="28" t="s">
+      <c r="C34" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="L34" s="17" t="s">
+      <c r="L34" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="M34" s="18"/>
+      <c r="M34" s="33"/>
     </row>
     <row r="35" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="29" t="s">
+      <c r="B35" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="C35" s="30" t="s">
+      <c r="C35" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="L35" s="19" t="s">
+      <c r="L35" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="M35" s="20"/>
+      <c r="M35" s="31"/>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B36" s="17" t="s">
+      <c r="B36" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="C36" s="18"/>
-      <c r="L36" s="21" t="s">
+      <c r="C36" s="33"/>
+      <c r="L36" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="M36" s="22"/>
+      <c r="M36" s="35"/>
     </row>
     <row r="37" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="19" t="s">
+      <c r="B37" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="C37" s="20"/>
-      <c r="L37" s="23" t="s">
+      <c r="C37" s="31"/>
+      <c r="L37" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="M37" s="24"/>
+      <c r="M37" s="37"/>
     </row>
     <row r="38" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="21" t="s">
+      <c r="B38" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="C38" s="22"/>
-      <c r="L38" s="25" t="s">
+      <c r="C38" s="35"/>
+      <c r="L38" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="M38" s="26"/>
+      <c r="M38" s="39"/>
     </row>
     <row r="39" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="23" t="s">
+      <c r="B39" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="C39" s="24"/>
-      <c r="L39" s="35" t="s">
+      <c r="C39" s="37"/>
+      <c r="L39" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="M39" s="36"/>
+      <c r="M39" s="41"/>
     </row>
     <row r="40" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="25" t="s">
+      <c r="B40" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="C40" s="26"/>
-      <c r="L40" s="37" t="s">
+      <c r="C40" s="39"/>
+      <c r="L40" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="M40" s="38"/>
+      <c r="M40" s="29"/>
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B41" s="40"/>
-      <c r="C41" s="40"/>
+      <c r="B41" s="46"/>
+      <c r="C41" s="46"/>
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B42" s="40"/>
-      <c r="C42" s="40"/>
+      <c r="B42" s="46"/>
+      <c r="C42" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="67">
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="L14:M14"/>
+    <mergeCell ref="L15:M15"/>
     <mergeCell ref="L40:M40"/>
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="B23:C23"/>
@@ -3010,57 +3101,694 @@
     <mergeCell ref="L19:M19"/>
     <mergeCell ref="L22:M22"/>
     <mergeCell ref="L23:M23"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L29" sqref="L29:M29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="6" style="24" customWidth="1"/>
+    <col min="2" max="2" width="25.77734375" style="24" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" style="24" customWidth="1"/>
+    <col min="4" max="4" width="32.6640625" style="24" customWidth="1"/>
+    <col min="5" max="6" width="8.88671875" style="24" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="4.109375" style="24" customWidth="1"/>
+    <col min="8" max="8" width="32.33203125" style="24" customWidth="1"/>
+    <col min="9" max="9" width="20.109375" style="24" customWidth="1"/>
+    <col min="10" max="10" width="45.88671875" style="24" customWidth="1"/>
+    <col min="11" max="11" width="6.21875" style="24" customWidth="1"/>
+    <col min="12" max="12" width="33.109375" style="24" customWidth="1"/>
+    <col min="13" max="13" width="23.5546875" style="24" customWidth="1"/>
+    <col min="14" max="16384" width="8.88671875" style="24"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="47" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="48"/>
+      <c r="H1" s="42" t="s">
+        <v>93</v>
+      </c>
+      <c r="I1" s="42"/>
+      <c r="L1" s="42" t="s">
+        <v>93</v>
+      </c>
+      <c r="M1" s="42"/>
+    </row>
+    <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="43" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" s="44"/>
+      <c r="H2" s="43" t="s">
+        <v>94</v>
+      </c>
+      <c r="I2" s="44"/>
+      <c r="L2" s="45" t="s">
+        <v>117</v>
+      </c>
+      <c r="M2" s="44"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="50" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="L3" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="M3" s="19" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="50" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="L4" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="M4" s="21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="50" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="H5" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="L5" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="M5" s="21" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="50" t="s">
+        <v>123</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="I6" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="L6" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="M6" s="21" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="50" t="s">
+        <v>123</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="33"/>
+      <c r="H7" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="I7" s="33"/>
+      <c r="L7" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="M7" s="25" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="50" t="s">
+        <v>123</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="31"/>
+      <c r="H8" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="I8" s="31"/>
+      <c r="L8" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="M8" s="21" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="50" t="s">
+        <v>123</v>
+      </c>
+      <c r="B9" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="35"/>
+      <c r="H9" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="I9" s="35"/>
+      <c r="L9" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="M9" s="21" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="50" t="s">
+        <v>123</v>
+      </c>
+      <c r="B10" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" s="37"/>
+      <c r="H10" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="I10" s="37"/>
+      <c r="L10" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="M10" s="21" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="50" t="s">
+        <v>123</v>
+      </c>
+      <c r="B11" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" s="39"/>
+      <c r="L11" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="M11" s="26" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B12" s="46"/>
+      <c r="C12" s="46"/>
+      <c r="L12" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="M12" s="33"/>
+    </row>
+    <row r="13" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="46"/>
+      <c r="C13" s="46"/>
+      <c r="H13" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="I13" s="42"/>
+      <c r="L13" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="M13" s="31"/>
+    </row>
+    <row r="14" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H14" s="45" t="s">
+        <v>98</v>
+      </c>
+      <c r="I14" s="44"/>
+      <c r="L14" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="M14" s="35"/>
+    </row>
+    <row r="15" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H15" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="I15" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="L15" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="M15" s="37"/>
+    </row>
+    <row r="16" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="47" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16" s="48"/>
+      <c r="H16" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="I16" s="21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="43" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" s="44"/>
+      <c r="H17" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="I17" s="21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="H18" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="I18" s="33"/>
+      <c r="L18" s="42" t="s">
+        <v>93</v>
+      </c>
+      <c r="M18" s="42"/>
+    </row>
+    <row r="19" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="H19" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="I19" s="31"/>
+      <c r="L19" s="43" t="s">
+        <v>116</v>
+      </c>
+      <c r="M19" s="44"/>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B20" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="H20" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="I20" s="35"/>
+      <c r="L20" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="M20" s="21" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="H21" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="I21" s="37"/>
+      <c r="L21" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="M21" s="21" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" s="33"/>
+      <c r="H22" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="I22" s="39"/>
+      <c r="L22" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="M22" s="33"/>
+    </row>
+    <row r="23" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="C23" s="31"/>
+      <c r="H23" s="40" t="s">
+        <v>74</v>
+      </c>
+      <c r="I23" s="41"/>
+      <c r="L23" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="M23" s="31"/>
+    </row>
+    <row r="24" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24" s="31"/>
+      <c r="H24" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="I24" s="29"/>
+      <c r="L24" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="M24" s="35"/>
+    </row>
+    <row r="25" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" s="35"/>
+      <c r="L25" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="M25" s="37"/>
+    </row>
+    <row r="26" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="C26" s="37"/>
+    </row>
+    <row r="27" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="38" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" s="39"/>
+      <c r="H27" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="I27" s="42"/>
+    </row>
+    <row r="28" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="46"/>
+      <c r="C28" s="46"/>
+      <c r="H28" s="43" t="s">
+        <v>102</v>
+      </c>
+      <c r="I28" s="44"/>
+      <c r="L28" s="42" t="s">
+        <v>104</v>
+      </c>
+      <c r="M28" s="42"/>
+    </row>
+    <row r="29" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="46"/>
+      <c r="C29" s="46"/>
+      <c r="H29" s="38" t="s">
+        <v>103</v>
+      </c>
+      <c r="I29" s="39"/>
+      <c r="L29" s="43" t="s">
+        <v>101</v>
+      </c>
+      <c r="M29" s="44"/>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="L30" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="M30" s="19" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L31" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="M31" s="21" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="47" t="s">
+        <v>92</v>
+      </c>
+      <c r="C32" s="48"/>
+      <c r="L32" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="M32" s="21" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="43" t="s">
+        <v>89</v>
+      </c>
+      <c r="C33" s="44"/>
+      <c r="L33" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="M33" s="23" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A34" s="50" t="s">
+        <v>123</v>
+      </c>
+      <c r="B34" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="L34" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="M34" s="33"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A35" s="50" t="s">
+        <v>123</v>
+      </c>
+      <c r="B35" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C35" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="L35" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="M35" s="31"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A36" s="50" t="s">
+        <v>123</v>
+      </c>
+      <c r="B36" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="L36" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="M36" s="35"/>
+    </row>
+    <row r="37" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="50" t="s">
+        <v>123</v>
+      </c>
+      <c r="B37" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="C37" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="L37" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="M37" s="37"/>
+    </row>
+    <row r="38" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="50" t="s">
+        <v>123</v>
+      </c>
+      <c r="B38" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="C38" s="33"/>
+      <c r="L38" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="M38" s="39"/>
+    </row>
+    <row r="39" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="50" t="s">
+        <v>123</v>
+      </c>
+      <c r="B39" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C39" s="31"/>
+      <c r="L39" s="40" t="s">
+        <v>74</v>
+      </c>
+      <c r="M39" s="41"/>
+    </row>
+    <row r="40" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="50" t="s">
+        <v>123</v>
+      </c>
+      <c r="B40" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="C40" s="35"/>
+      <c r="L40" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="M40" s="29"/>
+    </row>
+    <row r="41" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="50" t="s">
+        <v>123</v>
+      </c>
+      <c r="B41" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="C41" s="37"/>
+    </row>
+    <row r="42" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B42" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="C42" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="64">
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="L39:M39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="L40:M40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="L35:M35"/>
+    <mergeCell ref="L36:M36"/>
+    <mergeCell ref="L37:M37"/>
+    <mergeCell ref="L38:M38"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="L34:M34"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="L28:M28"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="H24:I24"/>
     <mergeCell ref="L24:M24"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="H14:I14"/>
     <mergeCell ref="L14:M14"/>
     <mergeCell ref="L15:M15"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="B13:C13"/>
     <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="B1:C1"/>
     <mergeCell ref="H1:I1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="B2:C2"/>
     <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="L2:M2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>